<commit_message>
correct kropt reduction times
</commit_message>
<xml_diff>
--- a/knn_results/kropt_reduction.xlsx
+++ b/knn_results/kropt_reduction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tair\PycharmProjects\MAI-IML-W3\knn_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{44305D86-D53C-4872-B3D1-E0693DA2BB52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{00DFD761-9BDF-45A8-9B87-7C0C0B3346DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -2526,14 +2526,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -2910,16 +2911,16 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2192</v>
+        <v>6.1446211338043204</v>
       </c>
       <c r="B21">
-        <v>2116</v>
+        <v>2000.1803841590799</v>
       </c>
       <c r="C21">
-        <v>2008</v>
+        <v>228.58463430404601</v>
       </c>
       <c r="D21">
-        <v>696</v>
+        <v>10.0875227451324</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>0</v>
@@ -2928,27 +2929,27 @@
         <v>10</v>
       </c>
       <c r="I21" s="1">
-        <v>22334</v>
+        <v>64.737321615219059</v>
       </c>
       <c r="J21" s="1">
-        <v>2233.4</v>
+        <v>6.4737321615219061</v>
       </c>
       <c r="K21" s="1">
-        <v>893.37777777777762</v>
+        <v>0.53369989482009339</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2224</v>
+        <v>5.94313168525695</v>
       </c>
       <c r="B22">
-        <v>2120</v>
+        <v>2532.5105450153301</v>
       </c>
       <c r="C22">
-        <v>2019</v>
+        <v>198.90165853500301</v>
       </c>
       <c r="D22">
-        <v>765</v>
+        <v>10.455570697784401</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>1</v>
@@ -2957,27 +2958,27 @@
         <v>10</v>
       </c>
       <c r="I22" s="1">
-        <v>21294</v>
+        <v>24019.945114850951</v>
       </c>
       <c r="J22" s="1">
-        <v>2129.4</v>
+        <v>2401.9945114850952</v>
       </c>
       <c r="K22" s="1">
-        <v>979.59999999999991</v>
+        <v>74800.016983884911</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2281</v>
+        <v>5.9491238594055096</v>
       </c>
       <c r="B23">
-        <v>2163</v>
+        <v>2707.3796503543799</v>
       </c>
       <c r="C23">
-        <v>2071</v>
+        <v>194.60154581069901</v>
       </c>
       <c r="D23">
-        <v>754</v>
+        <v>10.4448153972625</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>2</v>
@@ -2986,27 +2987,27 @@
         <v>10</v>
       </c>
       <c r="I23" s="1">
-        <v>20254</v>
+        <v>1916.4714722633319</v>
       </c>
       <c r="J23" s="1">
-        <v>2025.4</v>
+        <v>191.64714722633317</v>
       </c>
       <c r="K23" s="1">
-        <v>883.37777777777762</v>
+        <v>236.04030920619621</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>2208</v>
+        <v>5.97568488121032</v>
       </c>
       <c r="B24">
-        <v>2061</v>
+        <v>1974.6941828727699</v>
       </c>
       <c r="C24">
-        <v>1983</v>
+        <v>187.938019275665</v>
       </c>
       <c r="D24">
-        <v>761</v>
+        <v>10.471176624298</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>3</v>
@@ -3015,55 +3016,55 @@
         <v>10</v>
       </c>
       <c r="I24" s="2">
-        <v>7567</v>
+        <v>104.12640857696481</v>
       </c>
       <c r="J24" s="2">
-        <v>756.7</v>
+        <v>10.412640857696481</v>
       </c>
       <c r="K24" s="2">
-        <v>537.34444444444443</v>
+        <v>1.3450523444093844E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2217</v>
+        <v>6.0945928096771196</v>
       </c>
       <c r="B25">
-        <v>2132</v>
+        <v>2567.4352707862799</v>
       </c>
       <c r="C25">
-        <v>2019</v>
+        <v>190.35401844978301</v>
       </c>
       <c r="D25">
-        <v>784</v>
+        <v>10.433064699172901</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2245</v>
+        <v>6.0776596069335902</v>
       </c>
       <c r="B26">
-        <v>2154</v>
+        <v>2518.2201952934201</v>
       </c>
       <c r="C26">
-        <v>2007</v>
+        <v>196.90826129913299</v>
       </c>
       <c r="D26">
-        <v>764</v>
+        <v>10.4409625530242</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>2228</v>
+        <v>6.4992554187774596</v>
       </c>
       <c r="B27">
-        <v>2114</v>
+        <v>2282.8988213539101</v>
       </c>
       <c r="C27">
-        <v>2006</v>
+        <v>182.76189756393401</v>
       </c>
       <c r="D27">
-        <v>771</v>
+        <v>10.433826208114599</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -3071,16 +3072,16 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>2239</v>
+        <v>7.9892451763152996</v>
       </c>
       <c r="B28">
-        <v>2137</v>
+        <v>2302.8733179569199</v>
       </c>
       <c r="C28">
-        <v>2020</v>
+        <v>171.421284675598</v>
       </c>
       <c r="D28">
-        <v>753</v>
+        <v>10.448426485061599</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>12</v>
@@ -3106,34 +3107,34 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>2216</v>
+        <v>6.45373106002807</v>
       </c>
       <c r="B29">
-        <v>2125</v>
+        <v>2343.7110028266902</v>
       </c>
       <c r="C29">
-        <v>2045</v>
+        <v>182.22777366638101</v>
       </c>
       <c r="D29">
-        <v>756</v>
+        <v>10.4903218746185</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H29" s="1">
-        <v>14348609.675000001</v>
+        <v>41027424.434293725</v>
       </c>
       <c r="I29" s="1">
         <v>3</v>
       </c>
       <c r="J29" s="1">
-        <v>4782869.8916666666</v>
+        <v>13675808.144764574</v>
       </c>
       <c r="K29" s="1">
-        <v>5808.5070184493643</v>
+        <v>729.02062912827751</v>
       </c>
       <c r="L29" s="1">
-        <v>2.2106407280795898E-48</v>
+        <v>2.8440341794522369E-32</v>
       </c>
       <c r="M29" s="1">
         <v>2.8662655509401795</v>
@@ -3141,28 +3142,28 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>2284</v>
+        <v>7.6102759838104204</v>
       </c>
       <c r="B30">
-        <v>2172</v>
+        <v>2790.04174423217</v>
       </c>
       <c r="C30">
-        <v>2076</v>
+        <v>182.77237868309001</v>
       </c>
       <c r="D30">
-        <v>763</v>
+        <v>10.420721292495699</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H30" s="1">
-        <v>29643.299999999996</v>
+        <v>675329.43999160163</v>
       </c>
       <c r="I30" s="1">
         <v>36</v>
       </c>
       <c r="J30" s="1">
-        <v>823.42499999999984</v>
+        <v>18759.151110877821</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -3182,7 +3183,7 @@
         <v>21</v>
       </c>
       <c r="H32" s="2">
-        <v>14378252.975000001</v>
+        <v>41702753.874285325</v>
       </c>
       <c r="I32" s="2">
         <v>39</v>
@@ -3198,7 +3199,7 @@
     <mergeCell ref="A19:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:M16">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3209,7 +3210,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:M32">
+  <conditionalFormatting sqref="H20:M32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>